<commit_message>
BP-767: Fixed MANY bugs with initial db data
</commit_message>
<xml_diff>
--- a/assets/editor-names.xlsx
+++ b/assets/editor-names.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16160" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -3429,9 +3429,6 @@
     <t>Гимназия №1529 им. А.С.Грибоедова</t>
   </si>
   <si>
-    <t>Гимназия №12744 им. В.В.Маяковского</t>
-  </si>
-  <si>
     <t>Гимназия №1562 им. Артема Боровика</t>
   </si>
   <si>
@@ -3648,9 +3645,6 @@
     <t>Школа №1359 им. М.Л.Миля</t>
   </si>
   <si>
-    <t>ра</t>
-  </si>
-  <si>
     <t>Гимназия Марьина Роща им. В.Ф. Орлова</t>
   </si>
   <si>
@@ -3783,9 +3777,6 @@
     <t>Школа №460 им. А.А. Головачёва</t>
   </si>
   <si>
-    <t>Школа №463 им. Д.Н.Медведев</t>
-  </si>
-  <si>
     <t>Школа №479 им. В.И. Чуйкова</t>
   </si>
   <si>
@@ -3943,16 +3934,43 @@
   </si>
   <si>
     <t>Школа №1353 им. Д.Ф. Алексеева</t>
+  </si>
+  <si>
+    <t>Школа №1302</t>
+  </si>
+  <si>
+    <t>Школа №463 им. Д.Н.Медведева</t>
+  </si>
+  <si>
+    <t>Гимназия №1274 им. В.В.Маяковского</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -3976,15 +3994,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="2" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -4315,8 +4337,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D653"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A625" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4416,7 +4438,7 @@
         <v>458</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>1136</v>
+        <v>1307</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>12</v>
@@ -4542,7 +4564,7 @@
         <v>464</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>1278</v>
+        <v>1275</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>29</v>
@@ -4976,7 +4998,7 @@
         <v>106</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>88</v>
@@ -5158,7 +5180,7 @@
         <v>318</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>1279</v>
+        <v>1276</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>113</v>
@@ -5242,7 +5264,7 @@
         <v>153</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>124</v>
@@ -5382,7 +5404,7 @@
         <v>456</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>1280</v>
+        <v>1277</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>143</v>
@@ -5438,7 +5460,7 @@
         <v>476</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>150</v>
@@ -5480,7 +5502,7 @@
         <v>548</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>1210</v>
+        <v>1208</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>155</v>
@@ -5550,7 +5572,7 @@
         <v>579</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>1211</v>
+        <v>1209</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>164</v>
@@ -5564,7 +5586,7 @@
         <v>648</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>1281</v>
+        <v>1278</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>165</v>
@@ -5578,7 +5600,7 @@
         <v>647</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>1282</v>
+        <v>1279</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>166</v>
@@ -5648,7 +5670,7 @@
         <v>26</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>175</v>
@@ -5676,7 +5698,7 @@
         <v>124</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>178</v>
@@ -5690,7 +5712,7 @@
         <v>125</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>179</v>
@@ -5704,7 +5726,7 @@
         <v>268</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>180</v>
@@ -5760,7 +5782,7 @@
         <v>168</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>187</v>
@@ -5788,7 +5810,7 @@
         <v>216</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>190</v>
@@ -5802,7 +5824,7 @@
         <v>217</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>191</v>
@@ -5830,7 +5852,7 @@
         <v>123</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>194</v>
@@ -5914,7 +5936,7 @@
         <v>54</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>205</v>
@@ -5970,7 +5992,7 @@
         <v>565</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>212</v>
@@ -6054,7 +6076,7 @@
         <v>614</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="C124" s="1" t="s">
         <v>223</v>
@@ -6082,7 +6104,7 @@
         <v>179</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="C126" s="1" t="s">
         <v>226</v>
@@ -6180,7 +6202,7 @@
         <v>281</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>1283</v>
+        <v>1280</v>
       </c>
       <c r="C133" s="1" t="s">
         <v>239</v>
@@ -6194,7 +6216,7 @@
         <v>316</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="C134" s="1" t="s">
         <v>240</v>
@@ -6250,7 +6272,7 @@
         <v>582</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="C138" s="1" t="s">
         <v>247</v>
@@ -6320,7 +6342,7 @@
         <v>340</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="C143" s="1" t="s">
         <v>256</v>
@@ -6418,7 +6440,7 @@
         <v>588</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="C150" s="1" t="s">
         <v>269</v>
@@ -6488,7 +6510,7 @@
         <v>58</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="C155" s="1" t="s">
         <v>278</v>
@@ -6544,7 +6566,7 @@
         <v>529</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>1284</v>
+        <v>1281</v>
       </c>
       <c r="C159" s="1" t="s">
         <v>285</v>
@@ -6572,7 +6594,7 @@
         <v>70</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="C161" s="1" t="s">
         <v>288</v>
@@ -6600,7 +6622,7 @@
         <v>108</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="C163" s="1" t="s">
         <v>291</v>
@@ -6628,7 +6650,7 @@
         <v>385</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="C165" s="1" t="s">
         <v>294</v>
@@ -6642,7 +6664,7 @@
         <v>491</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="C166" s="1" t="s">
         <v>295</v>
@@ -6656,7 +6678,7 @@
         <v>32</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="C167" s="1" t="s">
         <v>296</v>
@@ -6670,7 +6692,7 @@
         <v>254</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="C168" s="1" t="s">
         <v>297</v>
@@ -6698,7 +6720,7 @@
         <v>573</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="C170" s="1" t="s">
         <v>300</v>
@@ -6712,7 +6734,7 @@
         <v>390</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="C171" s="1" t="s">
         <v>301</v>
@@ -6726,7 +6748,7 @@
         <v>504</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="C172" s="1" t="s">
         <v>302</v>
@@ -6740,7 +6762,7 @@
         <v>257</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="C173" s="1" t="s">
         <v>303</v>
@@ -6754,7 +6776,7 @@
         <v>455</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="C174" s="1" t="s">
         <v>304</v>
@@ -6768,7 +6790,7 @@
         <v>466</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="C175" s="1" t="s">
         <v>305</v>
@@ -6782,7 +6804,7 @@
         <v>524</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="C176" s="1" t="s">
         <v>306</v>
@@ -6796,7 +6818,7 @@
         <v>564</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="C177" s="1" t="s">
         <v>307</v>
@@ -6810,7 +6832,7 @@
         <v>516</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="C178" s="1" t="s">
         <v>308</v>
@@ -6824,7 +6846,7 @@
         <v>620</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="C179" s="1" t="s">
         <v>309</v>
@@ -6838,7 +6860,7 @@
         <v>255</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="C180" s="1" t="s">
         <v>310</v>
@@ -6852,7 +6874,7 @@
         <v>567</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="C181" s="1" t="s">
         <v>311</v>
@@ -6866,7 +6888,7 @@
         <v>258</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>1285</v>
+        <v>1282</v>
       </c>
       <c r="C182" s="1" t="s">
         <v>312</v>
@@ -6880,7 +6902,7 @@
         <v>494</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="C183" s="1" t="s">
         <v>313</v>
@@ -6894,7 +6916,7 @@
         <v>256</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="C184" s="1" t="s">
         <v>314</v>
@@ -6908,7 +6930,7 @@
         <v>492</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="C185" s="1" t="s">
         <v>315</v>
@@ -6922,7 +6944,7 @@
         <v>260</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="C186" s="1" t="s">
         <v>316</v>
@@ -6936,7 +6958,7 @@
         <v>637</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="C187" s="1" t="s">
         <v>317</v>
@@ -6950,7 +6972,7 @@
         <v>598</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="C188" s="1" t="s">
         <v>318</v>
@@ -6964,7 +6986,7 @@
         <v>581</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="C189" s="1" t="s">
         <v>319</v>
@@ -6978,7 +7000,7 @@
         <v>515</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
       <c r="C190" s="1" t="s">
         <v>320</v>
@@ -6992,7 +7014,7 @@
         <v>534</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="C191" s="1" t="s">
         <v>321</v>
@@ -7006,7 +7028,7 @@
         <v>546</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="C192" s="1" t="s">
         <v>322</v>
@@ -7020,7 +7042,7 @@
         <v>386</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="C193" s="1" t="s">
         <v>323</v>
@@ -7034,7 +7056,7 @@
         <v>585</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="C194" s="1" t="s">
         <v>324</v>
@@ -7048,7 +7070,7 @@
         <v>621</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="C195" s="1" t="s">
         <v>325</v>
@@ -7062,7 +7084,7 @@
         <v>533</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="C196" s="1" t="s">
         <v>326</v>
@@ -7076,7 +7098,7 @@
         <v>630</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="C197" s="1" t="s">
         <v>327</v>
@@ -7090,7 +7112,7 @@
         <v>432</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="C198" s="1" t="s">
         <v>328</v>
@@ -7118,7 +7140,7 @@
         <v>259</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="C200" s="1" t="s">
         <v>331</v>
@@ -7132,7 +7154,7 @@
         <v>599</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="C201" s="1" t="s">
         <v>332</v>
@@ -7146,7 +7168,7 @@
         <v>523</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="C202" s="1" t="s">
         <v>333</v>
@@ -7160,7 +7182,7 @@
         <v>501</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="C203" s="1" t="s">
         <v>334</v>
@@ -7174,7 +7196,7 @@
         <v>627</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="C204" s="1" t="s">
         <v>335</v>
@@ -7188,7 +7210,7 @@
         <v>549</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="C205" s="1" t="s">
         <v>336</v>
@@ -7356,7 +7378,7 @@
         <v>112</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="C217" s="1" t="s">
         <v>359</v>
@@ -7412,7 +7434,7 @@
         <v>475</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="C221" s="1" t="s">
         <v>366</v>
@@ -7482,7 +7504,7 @@
         <v>397</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>1286</v>
+        <v>1283</v>
       </c>
       <c r="C226" s="1" t="s">
         <v>375</v>
@@ -7594,7 +7616,7 @@
         <v>93</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="C234" s="1" t="s">
         <v>390</v>
@@ -7608,7 +7630,7 @@
         <v>195</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>1287</v>
+        <v>1284</v>
       </c>
       <c r="C235" s="1" t="s">
         <v>391</v>
@@ -7762,7 +7784,7 @@
         <v>94</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="C246" s="1" t="s">
         <v>412</v>
@@ -7888,7 +7910,7 @@
         <v>366</v>
       </c>
       <c r="B255" s="1" t="s">
-        <v>1288</v>
+        <v>1285</v>
       </c>
       <c r="C255" s="1" t="s">
         <v>429</v>
@@ -7944,7 +7966,7 @@
         <v>147</v>
       </c>
       <c r="B259" s="1" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="C259" s="1" t="s">
         <v>436</v>
@@ -7986,7 +8008,7 @@
         <v>575</v>
       </c>
       <c r="B262" s="1" t="s">
-        <v>1289</v>
+        <v>1286</v>
       </c>
       <c r="C262" s="1" t="s">
         <v>441</v>
@@ -8000,7 +8022,7 @@
         <v>431</v>
       </c>
       <c r="B263" s="1" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="C263" s="1" t="s">
         <v>442</v>
@@ -8014,7 +8036,7 @@
         <v>99</v>
       </c>
       <c r="B264" s="1" t="s">
-        <v>1290</v>
+        <v>1287</v>
       </c>
       <c r="C264" s="1" t="s">
         <v>443</v>
@@ -8028,7 +8050,7 @@
         <v>158</v>
       </c>
       <c r="B265" s="1" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="C265" s="1" t="s">
         <v>444</v>
@@ -8042,7 +8064,7 @@
         <v>530</v>
       </c>
       <c r="B266" s="1" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="C266" s="1" t="s">
         <v>445</v>
@@ -8056,7 +8078,7 @@
         <v>250</v>
       </c>
       <c r="B267" s="1" t="s">
-        <v>1291</v>
+        <v>1288</v>
       </c>
       <c r="C267" s="1" t="s">
         <v>446</v>
@@ -8084,7 +8106,7 @@
         <v>172</v>
       </c>
       <c r="B269" s="1" t="s">
-        <v>1292</v>
+        <v>1289</v>
       </c>
       <c r="C269" s="1" t="s">
         <v>449</v>
@@ -8098,7 +8120,7 @@
         <v>413</v>
       </c>
       <c r="B270" s="1" t="s">
-        <v>1293</v>
+        <v>1290</v>
       </c>
       <c r="C270" s="1" t="s">
         <v>450</v>
@@ -8112,7 +8134,7 @@
         <v>629</v>
       </c>
       <c r="B271" s="1" t="s">
-        <v>1294</v>
+        <v>1291</v>
       </c>
       <c r="C271" s="1" t="s">
         <v>451</v>
@@ -8126,7 +8148,7 @@
         <v>357</v>
       </c>
       <c r="B272" s="1" t="s">
-        <v>1295</v>
+        <v>1292</v>
       </c>
       <c r="C272" s="1" t="s">
         <v>452</v>
@@ -8140,7 +8162,7 @@
         <v>162</v>
       </c>
       <c r="B273" s="1" t="s">
-        <v>1296</v>
+        <v>1293</v>
       </c>
       <c r="C273" s="1" t="s">
         <v>453</v>
@@ -8154,7 +8176,7 @@
         <v>47</v>
       </c>
       <c r="B274" s="1" t="s">
-        <v>1297</v>
+        <v>1294</v>
       </c>
       <c r="C274" s="1" t="s">
         <v>454</v>
@@ -8168,7 +8190,7 @@
         <v>606</v>
       </c>
       <c r="B275" s="1" t="s">
-        <v>1298</v>
+        <v>1295</v>
       </c>
       <c r="C275" s="1" t="s">
         <v>455</v>
@@ -8182,7 +8204,7 @@
         <v>619</v>
       </c>
       <c r="B276" s="1" t="s">
-        <v>1299</v>
+        <v>1296</v>
       </c>
       <c r="C276" s="1" t="s">
         <v>456</v>
@@ -8196,7 +8218,7 @@
         <v>300</v>
       </c>
       <c r="B277" s="1" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="C277" s="1" t="s">
         <v>457</v>
@@ -8210,7 +8232,7 @@
         <v>536</v>
       </c>
       <c r="B278" s="1" t="s">
-        <v>1300</v>
+        <v>1297</v>
       </c>
       <c r="C278" s="1" t="s">
         <v>458</v>
@@ -8224,7 +8246,7 @@
         <v>241</v>
       </c>
       <c r="B279" s="1" t="s">
-        <v>1301</v>
+        <v>1298</v>
       </c>
       <c r="C279" s="1" t="s">
         <v>459</v>
@@ -8238,7 +8260,7 @@
         <v>625</v>
       </c>
       <c r="B280" s="1" t="s">
-        <v>1302</v>
+        <v>1299</v>
       </c>
       <c r="C280" s="1" t="s">
         <v>460</v>
@@ -8252,7 +8274,7 @@
         <v>553</v>
       </c>
       <c r="B281" s="1" t="s">
-        <v>1303</v>
+        <v>1300</v>
       </c>
       <c r="C281" s="1" t="s">
         <v>461</v>
@@ -8266,7 +8288,7 @@
         <v>242</v>
       </c>
       <c r="B282" s="1" t="s">
-        <v>1304</v>
+        <v>1301</v>
       </c>
       <c r="C282" s="1" t="s">
         <v>462</v>
@@ -8280,7 +8302,7 @@
         <v>556</v>
       </c>
       <c r="B283" s="1" t="s">
-        <v>1305</v>
+        <v>1302</v>
       </c>
       <c r="C283" s="1" t="s">
         <v>463</v>
@@ -8294,7 +8316,7 @@
         <v>616</v>
       </c>
       <c r="B284" s="1" t="s">
-        <v>1306</v>
+        <v>1303</v>
       </c>
       <c r="C284" s="1" t="s">
         <v>464</v>
@@ -8532,7 +8554,7 @@
         <v>416</v>
       </c>
       <c r="B301" s="1" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="C301" s="1" t="s">
         <v>497</v>
@@ -8546,7 +8568,7 @@
         <v>149</v>
       </c>
       <c r="B302" s="1" t="s">
-        <v>1209</v>
+        <v>1305</v>
       </c>
       <c r="C302" s="1" t="s">
         <v>498</v>
@@ -8714,7 +8736,7 @@
         <v>221</v>
       </c>
       <c r="B314" s="1" t="s">
-        <v>1307</v>
+        <v>1304</v>
       </c>
       <c r="C314" s="1" t="s">
         <v>521</v>
@@ -8770,7 +8792,7 @@
         <v>639</v>
       </c>
       <c r="B318" s="1" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="C318" s="1" t="s">
         <v>528</v>
@@ -8784,7 +8806,7 @@
         <v>574</v>
       </c>
       <c r="B319" s="1" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="C319" s="1" t="s">
         <v>529</v>
@@ -8980,7 +9002,7 @@
         <v>463</v>
       </c>
       <c r="B333" s="1" t="s">
-        <v>1212</v>
+        <v>1210</v>
       </c>
       <c r="C333" s="1" t="s">
         <v>556</v>
@@ -9036,7 +9058,7 @@
         <v>593</v>
       </c>
       <c r="B337" s="1" t="s">
-        <v>1222</v>
+        <v>1220</v>
       </c>
       <c r="C337" s="1" t="s">
         <v>563</v>
@@ -9218,7 +9240,7 @@
         <v>307</v>
       </c>
       <c r="B350" s="1" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="C350" s="1" t="s">
         <v>588</v>
@@ -9232,7 +9254,7 @@
         <v>465</v>
       </c>
       <c r="B351" s="1" t="s">
-        <v>1224</v>
+        <v>1222</v>
       </c>
       <c r="C351" s="1" t="s">
         <v>589</v>
@@ -9260,7 +9282,7 @@
         <v>436</v>
       </c>
       <c r="B353" s="1" t="s">
-        <v>1225</v>
+        <v>1223</v>
       </c>
       <c r="C353" s="1" t="s">
         <v>592</v>
@@ -9358,7 +9380,7 @@
         <v>409</v>
       </c>
       <c r="B360" s="1" t="s">
-        <v>1226</v>
+        <v>1224</v>
       </c>
       <c r="C360" s="1" t="s">
         <v>605</v>
@@ -9372,7 +9394,7 @@
         <v>509</v>
       </c>
       <c r="B361" s="1" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
       <c r="C361" s="1" t="s">
         <v>606</v>
@@ -9512,7 +9534,7 @@
         <v>410</v>
       </c>
       <c r="B371" s="1" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
       <c r="C371" s="1" t="s">
         <v>625</v>
@@ -9526,7 +9548,7 @@
         <v>652</v>
       </c>
       <c r="B372" s="1" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
       <c r="C372" s="1" t="s">
         <v>626</v>
@@ -9568,7 +9590,7 @@
         <v>400</v>
       </c>
       <c r="B375" s="1" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="C375" s="1" t="s">
         <v>631</v>
@@ -9610,7 +9632,7 @@
         <v>356</v>
       </c>
       <c r="B378" s="1" t="s">
-        <v>1230</v>
+        <v>1228</v>
       </c>
       <c r="C378" s="1" t="s">
         <v>636</v>
@@ -9694,7 +9716,7 @@
         <v>292</v>
       </c>
       <c r="B384" s="1" t="s">
-        <v>1214</v>
+        <v>1212</v>
       </c>
       <c r="C384" s="1" t="s">
         <v>647</v>
@@ -9750,7 +9772,7 @@
         <v>314</v>
       </c>
       <c r="B388" s="1" t="s">
-        <v>1231</v>
+        <v>1229</v>
       </c>
       <c r="C388" s="1" t="s">
         <v>654</v>
@@ -9904,7 +9926,7 @@
         <v>231</v>
       </c>
       <c r="B399" s="1" t="s">
-        <v>1232</v>
+        <v>1230</v>
       </c>
       <c r="C399" s="1" t="s">
         <v>675</v>
@@ -9974,7 +9996,7 @@
         <v>343</v>
       </c>
       <c r="B404" s="1" t="s">
-        <v>1233</v>
+        <v>1231</v>
       </c>
       <c r="C404" s="1" t="s">
         <v>684</v>
@@ -10058,7 +10080,7 @@
         <v>378</v>
       </c>
       <c r="B410" s="1" t="s">
-        <v>1234</v>
+        <v>1232</v>
       </c>
       <c r="C410" s="1" t="s">
         <v>695</v>
@@ -10072,7 +10094,7 @@
         <v>632</v>
       </c>
       <c r="B411" s="1" t="s">
-        <v>1269</v>
+        <v>1266</v>
       </c>
       <c r="C411" s="1" t="s">
         <v>696</v>
@@ -10212,7 +10234,7 @@
         <v>365</v>
       </c>
       <c r="B421" s="1" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="C421" s="1" t="s">
         <v>715</v>
@@ -10422,7 +10444,7 @@
         <v>157</v>
       </c>
       <c r="B436" s="1" t="s">
-        <v>1236</v>
+        <v>1234</v>
       </c>
       <c r="C436" s="1" t="s">
         <v>744</v>
@@ -10450,7 +10472,7 @@
         <v>327</v>
       </c>
       <c r="B438" s="1" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
       <c r="C438" s="1" t="s">
         <v>747</v>
@@ -10590,7 +10612,7 @@
         <v>160</v>
       </c>
       <c r="B448" s="1" t="s">
-        <v>1270</v>
+        <v>1267</v>
       </c>
       <c r="C448" s="1" t="s">
         <v>766</v>
@@ -10716,7 +10738,7 @@
         <v>331</v>
       </c>
       <c r="B457" s="1" t="s">
-        <v>1238</v>
+        <v>1236</v>
       </c>
       <c r="C457" s="1" t="s">
         <v>783</v>
@@ -10730,7 +10752,7 @@
         <v>603</v>
       </c>
       <c r="B458" s="1" t="s">
-        <v>1239</v>
+        <v>1237</v>
       </c>
       <c r="C458" s="1" t="s">
         <v>784</v>
@@ -10786,7 +10808,7 @@
         <v>338</v>
       </c>
       <c r="B462" s="1" t="s">
-        <v>1271</v>
+        <v>1268</v>
       </c>
       <c r="C462" s="1" t="s">
         <v>791</v>
@@ -10800,7 +10822,7 @@
         <v>348</v>
       </c>
       <c r="B463" s="1" t="s">
-        <v>1272</v>
+        <v>1269</v>
       </c>
       <c r="C463" s="1" t="s">
         <v>792</v>
@@ -10828,7 +10850,7 @@
         <v>345</v>
       </c>
       <c r="B465" s="1" t="s">
-        <v>1240</v>
+        <v>1238</v>
       </c>
       <c r="C465" s="1" t="s">
         <v>795</v>
@@ -10856,7 +10878,7 @@
         <v>586</v>
       </c>
       <c r="B467" s="1" t="s">
-        <v>1241</v>
+        <v>1239</v>
       </c>
       <c r="C467" s="1" t="s">
         <v>798</v>
@@ -10898,7 +10920,7 @@
         <v>411</v>
       </c>
       <c r="B470" s="1" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
       <c r="C470" s="1" t="s">
         <v>803</v>
@@ -10996,7 +11018,7 @@
         <v>460</v>
       </c>
       <c r="B477" s="1" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="C477" s="1" t="s">
         <v>816</v>
@@ -11052,7 +11074,7 @@
         <v>425</v>
       </c>
       <c r="B481" s="1" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
       <c r="C481" s="1" t="s">
         <v>823</v>
@@ -11066,7 +11088,7 @@
         <v>445</v>
       </c>
       <c r="B482" s="1" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="C482" s="1" t="s">
         <v>824</v>
@@ -11094,7 +11116,7 @@
         <v>541</v>
       </c>
       <c r="B484" s="1" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="C484" s="1" t="s">
         <v>827</v>
@@ -11136,7 +11158,7 @@
         <v>563</v>
       </c>
       <c r="B487" s="1" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="C487" s="1" t="s">
         <v>832</v>
@@ -11150,7 +11172,7 @@
         <v>559</v>
       </c>
       <c r="B488" s="1" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="C488" s="1" t="s">
         <v>833</v>
@@ -11262,7 +11284,7 @@
         <v>438</v>
       </c>
       <c r="B496" s="1" t="s">
-        <v>1273</v>
+        <v>1270</v>
       </c>
       <c r="C496" s="1" t="s">
         <v>848</v>
@@ -11276,7 +11298,7 @@
         <v>377</v>
       </c>
       <c r="B497" s="1" t="s">
-        <v>1274</v>
+        <v>1271</v>
       </c>
       <c r="C497" s="1" t="s">
         <v>849</v>
@@ -11346,7 +11368,7 @@
         <v>469</v>
       </c>
       <c r="B502" s="1" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="C502" s="1" t="s">
         <v>858</v>
@@ -11388,7 +11410,7 @@
         <v>358</v>
       </c>
       <c r="B505" s="1" t="s">
-        <v>1215</v>
+        <v>1213</v>
       </c>
       <c r="C505" s="1" t="s">
         <v>863</v>
@@ -11416,7 +11438,7 @@
         <v>286</v>
       </c>
       <c r="B507" s="1" t="s">
-        <v>1216</v>
+        <v>1214</v>
       </c>
       <c r="C507" s="1" t="s">
         <v>866</v>
@@ -11514,7 +11536,7 @@
         <v>351</v>
       </c>
       <c r="B514" s="1" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="C514" s="1" t="s">
         <v>879</v>
@@ -11542,7 +11564,7 @@
         <v>293</v>
       </c>
       <c r="B516" s="1" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="C516" s="1" t="s">
         <v>882</v>
@@ -11682,7 +11704,7 @@
         <v>446</v>
       </c>
       <c r="B526" s="1" t="s">
-        <v>1252</v>
+        <v>1250</v>
       </c>
       <c r="C526" s="1" t="s">
         <v>901</v>
@@ -11752,7 +11774,7 @@
         <v>602</v>
       </c>
       <c r="B531" s="1" t="s">
-        <v>1253</v>
+        <v>1251</v>
       </c>
       <c r="C531" s="1" t="s">
         <v>910</v>
@@ -11766,7 +11788,7 @@
         <v>429</v>
       </c>
       <c r="B532" s="1" t="s">
-        <v>1254</v>
+        <v>1306</v>
       </c>
       <c r="C532" s="1" t="s">
         <v>911</v>
@@ -11780,7 +11802,7 @@
         <v>82</v>
       </c>
       <c r="B533" s="1" t="s">
-        <v>1255</v>
+        <v>1252</v>
       </c>
       <c r="C533" s="1" t="s">
         <v>912</v>
@@ -11794,7 +11816,7 @@
         <v>161</v>
       </c>
       <c r="B534" s="1" t="s">
-        <v>1275</v>
+        <v>1272</v>
       </c>
       <c r="C534" s="1" t="s">
         <v>913</v>
@@ -11808,7 +11830,7 @@
         <v>78</v>
       </c>
       <c r="B535" s="1" t="s">
-        <v>1256</v>
+        <v>1253</v>
       </c>
       <c r="C535" s="1" t="s">
         <v>914</v>
@@ -11850,7 +11872,7 @@
         <v>507</v>
       </c>
       <c r="B538" s="1" t="s">
-        <v>1257</v>
+        <v>1254</v>
       </c>
       <c r="C538" s="1" t="s">
         <v>919</v>
@@ -11976,7 +11998,7 @@
         <v>391</v>
       </c>
       <c r="B547" s="1" t="s">
-        <v>1217</v>
+        <v>1215</v>
       </c>
       <c r="C547" s="1" t="s">
         <v>936</v>
@@ -12046,7 +12068,7 @@
         <v>5</v>
       </c>
       <c r="B552" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="C552" s="1" t="s">
         <v>945</v>
@@ -12060,7 +12082,7 @@
         <v>626</v>
       </c>
       <c r="B553" s="1" t="s">
-        <v>1259</v>
+        <v>1256</v>
       </c>
       <c r="C553" s="1" t="s">
         <v>946</v>
@@ -12158,7 +12180,7 @@
         <v>393</v>
       </c>
       <c r="B560" s="1" t="s">
-        <v>1276</v>
+        <v>1273</v>
       </c>
       <c r="C560" s="1" t="s">
         <v>959</v>
@@ -12214,7 +12236,7 @@
         <v>519</v>
       </c>
       <c r="B564" s="1" t="s">
-        <v>1260</v>
+        <v>1257</v>
       </c>
       <c r="C564" s="1" t="s">
         <v>966</v>
@@ -12256,7 +12278,7 @@
         <v>503</v>
       </c>
       <c r="B567" s="1" t="s">
-        <v>1218</v>
+        <v>1216</v>
       </c>
       <c r="C567" s="1" t="s">
         <v>971</v>
@@ -12284,7 +12306,7 @@
         <v>270</v>
       </c>
       <c r="B569" s="1" t="s">
-        <v>1219</v>
+        <v>1217</v>
       </c>
       <c r="C569" s="1" t="s">
         <v>974</v>
@@ -12298,7 +12320,7 @@
         <v>382</v>
       </c>
       <c r="B570" s="1" t="s">
-        <v>1220</v>
+        <v>1218</v>
       </c>
       <c r="C570" s="1" t="s">
         <v>975</v>
@@ -12354,7 +12376,7 @@
         <v>364</v>
       </c>
       <c r="B574" s="1" t="s">
-        <v>1261</v>
+        <v>1258</v>
       </c>
       <c r="C574" s="1" t="s">
         <v>982</v>
@@ -12396,7 +12418,7 @@
         <v>287</v>
       </c>
       <c r="B577" s="1" t="s">
-        <v>1221</v>
+        <v>1219</v>
       </c>
       <c r="C577" s="1" t="s">
         <v>987</v>
@@ -12536,7 +12558,7 @@
         <v>569</v>
       </c>
       <c r="B587" s="1" t="s">
-        <v>1262</v>
+        <v>1259</v>
       </c>
       <c r="C587" s="1" t="s">
         <v>1006</v>
@@ -12564,7 +12586,7 @@
         <v>528</v>
       </c>
       <c r="B589" s="1" t="s">
-        <v>1263</v>
+        <v>1260</v>
       </c>
       <c r="C589" s="1" t="s">
         <v>1009</v>
@@ -12858,7 +12880,7 @@
         <v>135</v>
       </c>
       <c r="B610" s="1" t="s">
-        <v>1264</v>
+        <v>1261</v>
       </c>
       <c r="C610" s="1" t="s">
         <v>1050</v>
@@ -12998,7 +13020,7 @@
         <v>136</v>
       </c>
       <c r="B620" s="1" t="s">
-        <v>1277</v>
+        <v>1274</v>
       </c>
       <c r="C620" s="1" t="s">
         <v>1069</v>
@@ -13054,7 +13076,7 @@
         <v>448</v>
       </c>
       <c r="B624" s="1" t="s">
-        <v>1265</v>
+        <v>1262</v>
       </c>
       <c r="C624" s="1" t="s">
         <v>1076</v>
@@ -13096,7 +13118,7 @@
         <v>645</v>
       </c>
       <c r="B627" s="1" t="s">
-        <v>1266</v>
+        <v>1263</v>
       </c>
       <c r="C627" s="1" t="s">
         <v>1081</v>
@@ -13194,7 +13216,7 @@
         <v>265</v>
       </c>
       <c r="B634" s="1" t="s">
-        <v>1267</v>
+        <v>1264</v>
       </c>
       <c r="C634" s="1" t="s">
         <v>1094</v>
@@ -13376,7 +13398,7 @@
         <v>274</v>
       </c>
       <c r="B647" s="1" t="s">
-        <v>1268</v>
+        <v>1265</v>
       </c>
       <c r="C647" s="1" t="s">
         <v>1119</v>
@@ -13471,6 +13493,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>